<commit_message>
fixing bugs - eventhandling
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\ISTER\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{33341918-CFC3-4DDB-B49F-024F774494BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9B66E745-4071-4FA4-819D-0E3DFFD10654}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Fehlerdokumentation von LitElement + warum wir jetzt Angular verwenden wollen</t>
+  </si>
+  <si>
+    <t>Mit Demo von Hr. Prof. Stütz Fehler gefixed</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +588,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>62</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1135,7 +1138,18 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
+      <c r="A43" s="2">
+        <v>43389</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>

</xml_diff>

<commit_message>
Added getAll to rest
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo3\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9B66E745-4071-4FA4-819D-0E3DFFD10654}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65877D0-C230-4D6B-8128-5840591D4E51}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
     <t>Datum</t>
   </si>
@@ -133,6 +138,9 @@
   </si>
   <si>
     <t>Mit Demo von Hr. Prof. Stütz Fehler gefixed</t>
+  </si>
+  <si>
+    <t>GetAll hinzugefügt</t>
   </si>
 </sst>
 </file>
@@ -522,16 +530,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="67.77734375" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +557,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43279</v>
       </c>
@@ -569,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43279</v>
       </c>
@@ -584,14 +592,14 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B150,"David",D2:D150)</f>
-        <v>40.5</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
         <v>63.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43296</v>
       </c>
@@ -605,7 +613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43296</v>
       </c>
@@ -619,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43311</v>
       </c>
@@ -633,7 +641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43311</v>
       </c>
@@ -647,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43326</v>
       </c>
@@ -661,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43326</v>
       </c>
@@ -675,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43328</v>
       </c>
@@ -689,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43331</v>
       </c>
@@ -703,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43332</v>
       </c>
@@ -717,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43333</v>
       </c>
@@ -731,7 +739,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43333</v>
       </c>
@@ -745,7 +753,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43334</v>
       </c>
@@ -759,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43336</v>
       </c>
@@ -773,7 +781,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43359</v>
       </c>
@@ -787,7 +795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43360</v>
       </c>
@@ -801,7 +809,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43360</v>
       </c>
@@ -815,7 +823,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43362</v>
       </c>
@@ -829,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43364</v>
       </c>
@@ -843,7 +851,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43365</v>
       </c>
@@ -857,7 +865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43366</v>
       </c>
@@ -871,7 +879,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43366</v>
       </c>
@@ -885,7 +893,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43366</v>
       </c>
@@ -899,7 +907,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43368</v>
       </c>
@@ -913,7 +921,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43368</v>
       </c>
@@ -927,7 +935,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43369</v>
       </c>
@@ -941,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43370</v>
       </c>
@@ -955,7 +963,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43371</v>
       </c>
@@ -969,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43373</v>
       </c>
@@ -983,7 +991,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43374</v>
       </c>
@@ -997,7 +1005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43374</v>
       </c>
@@ -1011,7 +1019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43375</v>
       </c>
@@ -1025,7 +1033,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43375</v>
       </c>
@@ -1039,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43376</v>
       </c>
@@ -1053,7 +1061,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43377</v>
       </c>
@@ -1067,7 +1075,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43378</v>
       </c>
@@ -1081,7 +1089,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43378</v>
       </c>
@@ -1095,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43380</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43381</v>
       </c>
@@ -1123,7 +1131,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43382</v>
       </c>
@@ -1137,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43389</v>
       </c>
@@ -1151,10 +1159,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43391</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added remaining GetAll Methods
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo3\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65877D0-C230-4D6B-8128-5840591D4E51}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC27403-AAF5-4877-80A2-501774AEBEDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -140,7 +140,7 @@
     <t>Mit Demo von Hr. Prof. Stütz Fehler gefixed</t>
   </si>
   <si>
-    <t>GetAll hinzugefügt</t>
+    <t>GetAll-Methoden finalisiert</t>
   </si>
 </sst>
 </file>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B150,"David",D2:D150)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
@@ -1170,7 +1170,7 @@
         <v>36</v>
       </c>
       <c r="D44">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked on post data
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo3\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC27403-AAF5-4877-80A2-501774AEBEDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FDDCDBC1-F694-4242-99EB-7F66C6B7E80D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -125,9 +120,6 @@
     <t>SQL-Statements für getAll() Methoden erstellt</t>
   </si>
   <si>
-    <t>POST Distance + Picture</t>
-  </si>
-  <si>
     <t>WebComponents mit Polymer 3, Fehler fixen</t>
   </si>
   <si>
@@ -141,6 +133,12 @@
   </si>
   <si>
     <t>GetAll-Methoden finalisiert</t>
+  </si>
+  <si>
+    <t>Website responsive gemacht, POST DataService</t>
+  </si>
+  <si>
+    <t>POST DataService</t>
   </si>
 </sst>
 </file>
@@ -530,16 +528,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="67.7109375" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +555,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43279</v>
       </c>
@@ -577,7 +575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43279</v>
       </c>
@@ -596,10 +594,10 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>63.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43296</v>
       </c>
@@ -613,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43296</v>
       </c>
@@ -627,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43311</v>
       </c>
@@ -641,7 +639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43311</v>
       </c>
@@ -655,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43326</v>
       </c>
@@ -669,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43326</v>
       </c>
@@ -683,7 +681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43328</v>
       </c>
@@ -697,7 +695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43331</v>
       </c>
@@ -711,7 +709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43332</v>
       </c>
@@ -725,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43333</v>
       </c>
@@ -739,7 +737,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43333</v>
       </c>
@@ -753,7 +751,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43334</v>
       </c>
@@ -767,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43336</v>
       </c>
@@ -781,7 +779,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43359</v>
       </c>
@@ -795,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43360</v>
       </c>
@@ -809,7 +807,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43360</v>
       </c>
@@ -823,7 +821,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43362</v>
       </c>
@@ -837,7 +835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43364</v>
       </c>
@@ -851,7 +849,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43365</v>
       </c>
@@ -865,7 +863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43366</v>
       </c>
@@ -879,7 +877,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43366</v>
       </c>
@@ -893,7 +891,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43366</v>
       </c>
@@ -907,7 +905,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43368</v>
       </c>
@@ -921,7 +919,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43368</v>
       </c>
@@ -935,7 +933,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43369</v>
       </c>
@@ -943,13 +941,13 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43370</v>
       </c>
@@ -957,13 +955,13 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29">
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43371</v>
       </c>
@@ -977,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43373</v>
       </c>
@@ -991,7 +989,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43374</v>
       </c>
@@ -1005,7 +1003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43374</v>
       </c>
@@ -1019,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43375</v>
       </c>
@@ -1033,7 +1031,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43375</v>
       </c>
@@ -1047,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>43376</v>
       </c>
@@ -1055,13 +1053,13 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36">
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>43377</v>
       </c>
@@ -1075,7 +1073,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>43378</v>
       </c>
@@ -1083,13 +1081,13 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38">
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43378</v>
       </c>
@@ -1103,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>43380</v>
       </c>
@@ -1117,23 +1115,23 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>43381</v>
+        <v>43382</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D41">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>43382</v>
+        <v>43389</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
@@ -1142,24 +1140,24 @@
         <v>34</v>
       </c>
       <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>43389</v>
+        <v>43391</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D43">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43391</v>
       </c>
@@ -1167,14 +1165,25 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44">
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>43394</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
finished post, excel reading
start pdf creating
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{04662BE3-FF5A-48A8-8006-F8B27AA0C492}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A28DC6E-7BE8-4C87-8B5C-E645128C75EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
   <si>
     <t>Datum</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>POST DataService</t>
+  </si>
+  <si>
+    <t>Bulk Upload Excel</t>
   </si>
 </sst>
 </file>
@@ -526,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +597,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>69.5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1197,6 +1200,20 @@
       </c>
       <c r="D46">
         <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>43402</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further working on design
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{81BD2CE4-3BFB-44C1-B1A3-C99CA0530036}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{174B296B-7975-4F96-94E3-A3A6809BBC99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <t>POST DataService</t>
   </si>
   <si>
-    <t>Read + POST Excel, using jsPdf, output Pdf, TestClientTester erweiter</t>
+    <t>Read + POST Excel, using jsPdf, output Pdf, TestClientTester erweitert, OverviewSelection</t>
   </si>
 </sst>
 </file>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,7 +597,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>77.5</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1213,7 +1213,7 @@
         <v>38</v>
       </c>
       <c r="D47">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited Tables(Foreign keys, auto increment) + backup.sql
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo3\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3ABC34-1D5C-472A-933F-4B22FDF68035}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF6CAD1-4FB6-451D-B35E-B8881D76081F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
   <si>
     <t>Datum</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Csv-Bulk Upload 1. Prototyp</t>
+  </si>
+  <si>
+    <t>Added Foreign Key to Database + Auto Increments + Backup.sql generated</t>
   </si>
 </sst>
 </file>
@@ -540,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +607,7 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B150,"David",D2:D150)</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
@@ -1252,6 +1255,20 @@
         <v>40</v>
       </c>
       <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>43404</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added pdf output for categories
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo4\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45DF48D-1AD2-498E-BCEC-524BAA342671}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B26C765-E643-4BA8-A5A7-8125AD697C9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -159,6 +154,9 @@
   </si>
   <si>
     <t>Besprechung Zusammenlegung FrontEnd/Backend</t>
+  </si>
+  <si>
+    <t>pdf-Ausgabe von Categories hinzugefügt</t>
   </si>
 </sst>
 </file>
@@ -549,15 +547,15 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="67.7109375" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +573,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43279</v>
       </c>
@@ -595,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43279</v>
       </c>
@@ -614,10 +612,10 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>87.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43296</v>
       </c>
@@ -631,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43296</v>
       </c>
@@ -645,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43311</v>
       </c>
@@ -659,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43311</v>
       </c>
@@ -673,7 +671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43326</v>
       </c>
@@ -687,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43326</v>
       </c>
@@ -701,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43328</v>
       </c>
@@ -715,7 +713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43331</v>
       </c>
@@ -729,7 +727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43332</v>
       </c>
@@ -743,7 +741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43333</v>
       </c>
@@ -757,7 +755,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43333</v>
       </c>
@@ -771,7 +769,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43334</v>
       </c>
@@ -785,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43336</v>
       </c>
@@ -799,7 +797,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43359</v>
       </c>
@@ -813,7 +811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43360</v>
       </c>
@@ -827,7 +825,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43360</v>
       </c>
@@ -841,7 +839,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43362</v>
       </c>
@@ -855,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43364</v>
       </c>
@@ -869,7 +867,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43365</v>
       </c>
@@ -883,7 +881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43366</v>
       </c>
@@ -897,7 +895,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43366</v>
       </c>
@@ -911,7 +909,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43366</v>
       </c>
@@ -925,7 +923,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43368</v>
       </c>
@@ -939,7 +937,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43368</v>
       </c>
@@ -953,7 +951,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43369</v>
       </c>
@@ -967,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43370</v>
       </c>
@@ -981,7 +979,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43371</v>
       </c>
@@ -995,7 +993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43373</v>
       </c>
@@ -1009,7 +1007,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43374</v>
       </c>
@@ -1023,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43374</v>
       </c>
@@ -1037,7 +1035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43375</v>
       </c>
@@ -1051,7 +1049,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43375</v>
       </c>
@@ -1065,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>43376</v>
       </c>
@@ -1079,7 +1077,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>43377</v>
       </c>
@@ -1093,7 +1091,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>43378</v>
       </c>
@@ -1107,7 +1105,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43378</v>
       </c>
@@ -1121,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>43380</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>43382</v>
       </c>
@@ -1149,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>43389</v>
       </c>
@@ -1163,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>43391</v>
       </c>
@@ -1177,7 +1175,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43391</v>
       </c>
@@ -1191,7 +1189,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43394</v>
       </c>
@@ -1205,7 +1203,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>43401</v>
       </c>
@@ -1219,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>43402</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>43403</v>
       </c>
@@ -1247,7 +1245,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>43404</v>
       </c>
@@ -1261,7 +1259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>43404</v>
       </c>
@@ -1275,7 +1273,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>43407</v>
       </c>
@@ -1289,7 +1287,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>43407</v>
       </c>
@@ -1303,8 +1301,19 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>43416</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53">
+        <v>2.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
further changes for pdf ouput
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B26C765-E643-4BA8-A5A7-8125AD697C9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{14015BEF-6E86-4ECC-B53C-D2A32BE8D7A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>90</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
         <v>43</v>
       </c>
       <c r="D53">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pdfCreator for logic separation
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{82FE1A7F-BF5D-4B31-A08A-1317581E993D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E595100-3EB1-4152-8472-3B5BFBF6AD50}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>WebsiteCountdown, pdf Output verfeinert, autpaging, page numbering, reworked testserver</t>
+  </si>
+  <si>
+    <t>Reworking Layers Separation</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +618,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>93.5</v>
+        <v>100.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1344,6 +1347,34 @@
       </c>
       <c r="D55">
         <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>43417</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>43418</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BIG FAT htdocs update + Arbeitszeiten
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo5\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FC0B706-1D3B-4F72-87F3-E674C6FA7CCD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B471A86B-DD09-447A-B8BE-540161646332}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="48">
   <si>
     <t>Datum</t>
   </si>
@@ -556,18 +561,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +590,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43279</v>
       </c>
@@ -605,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43279</v>
       </c>
@@ -620,14 +625,14 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B150,"David",D2:D150)</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43296</v>
       </c>
@@ -641,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43296</v>
       </c>
@@ -655,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43311</v>
       </c>
@@ -669,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43311</v>
       </c>
@@ -683,7 +688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43326</v>
       </c>
@@ -697,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43326</v>
       </c>
@@ -711,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43328</v>
       </c>
@@ -725,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43331</v>
       </c>
@@ -739,7 +744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43332</v>
       </c>
@@ -753,7 +758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43333</v>
       </c>
@@ -767,7 +772,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43333</v>
       </c>
@@ -781,7 +786,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43334</v>
       </c>
@@ -795,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43336</v>
       </c>
@@ -809,7 +814,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43359</v>
       </c>
@@ -823,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43360</v>
       </c>
@@ -837,7 +842,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43360</v>
       </c>
@@ -851,7 +856,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43362</v>
       </c>
@@ -865,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43364</v>
       </c>
@@ -879,7 +884,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43365</v>
       </c>
@@ -893,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43366</v>
       </c>
@@ -907,7 +912,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43366</v>
       </c>
@@ -921,7 +926,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43366</v>
       </c>
@@ -935,7 +940,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43368</v>
       </c>
@@ -949,7 +954,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43368</v>
       </c>
@@ -963,7 +968,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43369</v>
       </c>
@@ -977,7 +982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43370</v>
       </c>
@@ -991,7 +996,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43371</v>
       </c>
@@ -1005,7 +1010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43373</v>
       </c>
@@ -1019,7 +1024,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43374</v>
       </c>
@@ -1033,7 +1038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43374</v>
       </c>
@@ -1047,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43375</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43375</v>
       </c>
@@ -1075,7 +1080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43376</v>
       </c>
@@ -1089,7 +1094,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43377</v>
       </c>
@@ -1103,7 +1108,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43378</v>
       </c>
@@ -1117,7 +1122,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43378</v>
       </c>
@@ -1131,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43380</v>
       </c>
@@ -1145,7 +1150,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43382</v>
       </c>
@@ -1159,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43389</v>
       </c>
@@ -1173,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43391</v>
       </c>
@@ -1187,7 +1192,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43391</v>
       </c>
@@ -1201,7 +1206,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43394</v>
       </c>
@@ -1215,7 +1220,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43401</v>
       </c>
@@ -1229,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43402</v>
       </c>
@@ -1243,7 +1248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43403</v>
       </c>
@@ -1257,7 +1262,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43404</v>
       </c>
@@ -1271,7 +1276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43404</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43407</v>
       </c>
@@ -1299,7 +1304,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43407</v>
       </c>
@@ -1313,7 +1318,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43415</v>
       </c>
@@ -1327,7 +1332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43416</v>
       </c>
@@ -1341,7 +1346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43416</v>
       </c>
@@ -1355,7 +1360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43417</v>
       </c>
@@ -1369,7 +1374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43418</v>
       </c>
@@ -1383,7 +1388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43419</v>
       </c>
@@ -1397,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43419</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43420</v>
       </c>
@@ -1423,6 +1428,48 @@
       </c>
       <c r="D60">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>43419</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>43421</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>43422</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some more work hours
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{08E09C2F-07C7-4A16-9EA3-27D5A3DA64BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5637E691-FC15-4213-A452-BEB97B1CC5E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="49">
   <si>
     <t>Datum</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +627,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B150,"Daniel",D2:D150)</f>
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1525,6 +1525,51 @@
       <c r="D67">
         <v>3</v>
       </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>43441</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>48</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>43445</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed encoding + little frontend "bug"
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo5\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{07600B94-EC27-4FC5-B5C9-A860DDBCFAAC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F773AB49-E887-4B7B-B353-43EE3754D918}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="55">
   <si>
     <t>Datum</t>
   </si>
@@ -181,6 +187,15 @@
   </si>
   <si>
     <t>Reworked ChallengeCreator to ChallengeManager, added CRUD Functionality</t>
+  </si>
+  <si>
+    <t>Encoding fixes</t>
+  </si>
+  <si>
+    <t>Testing + fixing</t>
+  </si>
+  <si>
+    <t>Protokoll</t>
   </si>
 </sst>
 </file>
@@ -568,18 +583,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +612,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43279</v>
       </c>
@@ -617,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43279</v>
       </c>
@@ -632,14 +647,14 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B149,"David",D2:D149)</f>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
         <v>136.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43296</v>
       </c>
@@ -653,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43296</v>
       </c>
@@ -667,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43311</v>
       </c>
@@ -681,7 +696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43311</v>
       </c>
@@ -695,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43326</v>
       </c>
@@ -709,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43326</v>
       </c>
@@ -723,7 +738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43328</v>
       </c>
@@ -737,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43331</v>
       </c>
@@ -751,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43332</v>
       </c>
@@ -765,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43333</v>
       </c>
@@ -779,7 +794,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43333</v>
       </c>
@@ -793,7 +808,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43334</v>
       </c>
@@ -807,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43336</v>
       </c>
@@ -821,7 +836,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43359</v>
       </c>
@@ -835,7 +850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43360</v>
       </c>
@@ -849,7 +864,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43360</v>
       </c>
@@ -863,7 +878,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43362</v>
       </c>
@@ -877,7 +892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43364</v>
       </c>
@@ -891,7 +906,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43365</v>
       </c>
@@ -905,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43366</v>
       </c>
@@ -919,7 +934,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43366</v>
       </c>
@@ -933,7 +948,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43366</v>
       </c>
@@ -947,7 +962,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43368</v>
       </c>
@@ -961,7 +976,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43368</v>
       </c>
@@ -975,7 +990,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43369</v>
       </c>
@@ -989,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43370</v>
       </c>
@@ -1003,7 +1018,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43371</v>
       </c>
@@ -1017,7 +1032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43373</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43374</v>
       </c>
@@ -1045,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43374</v>
       </c>
@@ -1059,7 +1074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43375</v>
       </c>
@@ -1073,7 +1088,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43375</v>
       </c>
@@ -1087,7 +1102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43376</v>
       </c>
@@ -1101,7 +1116,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43377</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43378</v>
       </c>
@@ -1129,7 +1144,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43378</v>
       </c>
@@ -1143,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43380</v>
       </c>
@@ -1157,7 +1172,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43382</v>
       </c>
@@ -1171,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43389</v>
       </c>
@@ -1185,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43391</v>
       </c>
@@ -1199,7 +1214,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43391</v>
       </c>
@@ -1213,7 +1228,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43394</v>
       </c>
@@ -1227,7 +1242,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43401</v>
       </c>
@@ -1241,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43402</v>
       </c>
@@ -1255,7 +1270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43403</v>
       </c>
@@ -1269,7 +1284,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43404</v>
       </c>
@@ -1283,7 +1298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43404</v>
       </c>
@@ -1297,7 +1312,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43407</v>
       </c>
@@ -1311,7 +1326,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43407</v>
       </c>
@@ -1325,7 +1340,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43415</v>
       </c>
@@ -1339,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43416</v>
       </c>
@@ -1353,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43416</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43417</v>
       </c>
@@ -1381,7 +1396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43418</v>
       </c>
@@ -1395,7 +1410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43419</v>
       </c>
@@ -1409,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43419</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43420</v>
       </c>
@@ -1437,7 +1452,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>43419</v>
       </c>
@@ -1451,7 +1466,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43421</v>
       </c>
@@ -1465,7 +1480,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>43422</v>
       </c>
@@ -1479,7 +1494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>43424</v>
       </c>
@@ -1493,37 +1508,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
+        <v>43431</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>43435</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>54</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
         <v>43433</v>
-      </c>
-      <c r="B65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>43434</v>
-      </c>
-      <c r="B66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>43435</v>
       </c>
       <c r="B67" t="s">
         <v>3</v>
@@ -1535,9 +1550,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>43441</v>
+        <v>43434</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
@@ -1546,12 +1561,12 @@
         <v>48</v>
       </c>
       <c r="D68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>43444</v>
+        <v>43435</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
@@ -1563,46 +1578,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
+        <v>43441</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>48</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>43446</v>
       </c>
-      <c r="B70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
         <v>49</v>
       </c>
-      <c r="D70">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+      <c r="D72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>43447</v>
       </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
         <v>50</v>
       </c>
-      <c r="D71">
+      <c r="D73">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>43448</v>
       </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
         <v>51</v>
       </c>
-      <c r="D72">
+      <c r="D74">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>43448</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started with translation in languages
first step will be english+german without dropdown
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6DDE09C1-D303-4285-8639-73388C191273}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{13BEE5F3-6057-47A5-B446-11C57F6387B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="60">
   <si>
     <t>Datum</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>optionales Beweisbild, Beweisbildsuche, dynamische Challengeliste, EmailName Btn</t>
+  </si>
+  <si>
+    <t>erstellen der Daten für KV-Language-Table</t>
   </si>
 </sst>
 </file>
@@ -589,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,7 +660,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>151</v>
+        <v>152.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1722,6 +1725,20 @@
       </c>
       <c r="D79">
         <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>43455</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added work hours, reworked login-btn
and some more minor changes
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{13BEE5F3-6057-47A5-B446-11C57F6387B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7D8E8CE1-172F-4FE7-9EFB-ACB1A82D5DCC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>erstellen der Daten für KV-Language-Table</t>
+  </si>
+  <si>
+    <t>Skype-Konferenz, Besprechung der bevorstehenden Tasks</t>
+  </si>
+  <si>
+    <t>Zeitenprotokoll aktualisiert, Pop-Up für ändern von SessionDate, KV-Translation docx</t>
   </si>
 </sst>
 </file>
@@ -592,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,11 +662,11 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B149,"David",D2:D149)</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>152.5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1739,6 +1745,48 @@
       </c>
       <c r="D80">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>43458</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>43458</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>43458</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started multi languaging for first components
overviewselector, homeview, websiteheader, rankings
also added work hours
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7D8E8CE1-172F-4FE7-9EFB-ACB1A82D5DCC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1079F781-0EE9-4645-8374-A1D7738F4379}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="63">
   <si>
     <t>Datum</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Zeitenprotokoll aktualisiert, Pop-Up für ändern von SessionDate, KV-Translation docx</t>
+  </si>
+  <si>
+    <t>Translation Service</t>
   </si>
 </sst>
 </file>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +669,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>157</v>
+        <v>161.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1787,6 +1790,20 @@
       </c>
       <c r="D83">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>43459</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
translation for last component
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1079F781-0EE9-4645-8374-A1D7738F4379}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2B9D6B8A-0478-42AF-ADCB-5E2B76EEC076}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
   <si>
     <t>Datum</t>
   </si>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +669,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>161.5</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1804,6 +1804,20 @@
       </c>
       <c r="D84">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>43460</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started with club statistics tables
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2B9D6B8A-0478-42AF-ADCB-5E2B76EEC076}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3A2D3EFD-47C1-4568-9411-E4D01005ED5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
   <si>
     <t>Datum</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Translation Service</t>
+  </si>
+  <si>
+    <t>Code improvement, pdf Club</t>
   </si>
 </sst>
 </file>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +672,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1794,7 +1797,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
-        <v>43459</v>
+        <v>43460</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
@@ -1808,7 +1811,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
-        <v>43460</v>
+        <v>43462</v>
       </c>
       <c r="B85" t="s">
         <v>3</v>
@@ -1818,6 +1821,20 @@
       </c>
       <c r="D85">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <v>43463</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>63</v>
+      </c>
+      <c r="D86">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added work hours and tasks
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6D85B0C9-C49E-4DCC-8831-EA301FD47F49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{99100506-76D9-41F8-9EE8-A134CF5C24A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="67">
   <si>
     <t>Datum</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Code Review</t>
+  </si>
+  <si>
+    <t>reworked DataService, finished Challenge Manager</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +681,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1869,6 +1872,20 @@
       </c>
       <c r="D88">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>43103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixing challenge manager
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C5214778-90FB-40E4-92AC-E0A51D1B671B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70054CA2-D685-415E-90C6-F9C3EBD8248F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="68">
   <si>
     <t>Datum</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>reworked DataService, finished Challenge Manager, Debugging</t>
+  </si>
+  <si>
+    <t>Bug Fixing Challenge Manager, Code Review</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,12 +679,12 @@
         <v>3</v>
       </c>
       <c r="G3" s="4">
-        <f>SUMIF(B2:B149,"David",D2:D149)</f>
+        <f>SUMIF(B2:B200,"David",D2:D200)</f>
         <v>89</v>
       </c>
       <c r="H3">
-        <f>SUMIF(B2:B149,"Daniel",D2:D149)</f>
-        <v>183.5</v>
+        <f>SUMIF(B2:B200,"Daniel",D2:D200)</f>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1886,6 +1889,20 @@
       </c>
       <c r="D89">
         <v>6.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>43104</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" t="s">
+        <v>67</v>
+      </c>
+      <c r="D90">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing email logic reactions
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C9577616-563D-45D2-9EB9-208846ECEEF3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{802E187D-EC3E-422A-8AFB-FF62C56BA6BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Merged Google Signin + Bug fixing</t>
+  </si>
+  <si>
+    <t>Merged Google Signin + Bug fixing, implementing button visibilities</t>
   </si>
 </sst>
 </file>
@@ -622,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,7 +693,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B201,"Daniel",D2:D201)</f>
-        <v>189</v>
+        <v>190.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1947,11 +1950,14 @@
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D93">
-        <v>2</v>
-      </c>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added work hours, removed task
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2ABFC4-9CD3-4C8E-8452-0AA56DEB85FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70CA7A-9D13-4FC0-8570-6C783754C56E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -245,7 +245,7 @@
     <t>Merged Google Signin + Bug fixing, implementing button visibilities</t>
   </si>
   <si>
-    <t>Code Review, Background Images</t>
+    <t>Code Review, Background Images, Flag Dropdown</t>
   </si>
 </sst>
 </file>
@@ -636,7 +636,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B201,"Daniel",D2:D201)</f>
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1975,7 +1975,7 @@
         <v>71</v>
       </c>
       <c r="D94">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
email check + full backend translation service
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DaRepo7\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70CA7A-9D13-4FC0-8570-6C783754C56E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DA6ACD-6B6C-4F98-B813-CE72418F62D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="74">
   <si>
     <t>Datum</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>Code Review, Background Images, Flag Dropdown</t>
+  </si>
+  <si>
+    <t>Translation.csv erstellen + Translation in Db einspeisen</t>
+  </si>
+  <si>
+    <t>Algorithmus für Translation + Englisch Übersetzung</t>
   </si>
 </sst>
 </file>
@@ -633,18 +640,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4D4F47-197B-4479-93DD-E9C21F2B9FCB}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="70.33203125" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +669,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43279</v>
       </c>
@@ -682,7 +689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43279</v>
       </c>
@@ -697,14 +704,14 @@
       </c>
       <c r="G3" s="4">
         <f>SUMIF(B2:B201,"David",D2:D201)</f>
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="H3">
         <f>SUMIF(B2:B201,"Daniel",D2:D201)</f>
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43296</v>
       </c>
@@ -718,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43296</v>
       </c>
@@ -732,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43311</v>
       </c>
@@ -746,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43311</v>
       </c>
@@ -760,7 +767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43326</v>
       </c>
@@ -774,7 +781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43326</v>
       </c>
@@ -788,7 +795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43328</v>
       </c>
@@ -802,7 +809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43331</v>
       </c>
@@ -816,7 +823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43332</v>
       </c>
@@ -830,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43333</v>
       </c>
@@ -844,7 +851,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43333</v>
       </c>
@@ -858,7 +865,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43334</v>
       </c>
@@ -872,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43336</v>
       </c>
@@ -886,7 +893,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43359</v>
       </c>
@@ -900,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43360</v>
       </c>
@@ -914,7 +921,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43360</v>
       </c>
@@ -928,7 +935,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43362</v>
       </c>
@@ -942,7 +949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43364</v>
       </c>
@@ -956,7 +963,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43365</v>
       </c>
@@ -970,7 +977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43366</v>
       </c>
@@ -984,7 +991,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43366</v>
       </c>
@@ -998,7 +1005,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43366</v>
       </c>
@@ -1012,7 +1019,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43368</v>
       </c>
@@ -1026,7 +1033,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43368</v>
       </c>
@@ -1040,7 +1047,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43369</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43370</v>
       </c>
@@ -1068,7 +1075,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43371</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43373</v>
       </c>
@@ -1096,7 +1103,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43374</v>
       </c>
@@ -1110,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43374</v>
       </c>
@@ -1124,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43375</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43375</v>
       </c>
@@ -1152,7 +1159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43376</v>
       </c>
@@ -1166,7 +1173,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43377</v>
       </c>
@@ -1180,7 +1187,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43378</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43378</v>
       </c>
@@ -1208,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43380</v>
       </c>
@@ -1222,7 +1229,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43382</v>
       </c>
@@ -1236,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43389</v>
       </c>
@@ -1250,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43391</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43391</v>
       </c>
@@ -1278,7 +1285,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43394</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43401</v>
       </c>
@@ -1306,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43402</v>
       </c>
@@ -1320,7 +1327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43403</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43404</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43404</v>
       </c>
@@ -1362,7 +1369,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43407</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43407</v>
       </c>
@@ -1390,7 +1397,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43415</v>
       </c>
@@ -1404,7 +1411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43416</v>
       </c>
@@ -1418,7 +1425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43416</v>
       </c>
@@ -1432,7 +1439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43417</v>
       </c>
@@ -1446,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43418</v>
       </c>
@@ -1460,7 +1467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43419</v>
       </c>
@@ -1474,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43419</v>
       </c>
@@ -1488,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43420</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>43419</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43421</v>
       </c>
@@ -1530,7 +1537,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>43422</v>
       </c>
@@ -1544,7 +1551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>43424</v>
       </c>
@@ -1558,7 +1565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>43431</v>
       </c>
@@ -1572,7 +1579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>43435</v>
       </c>
@@ -1586,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>43433</v>
       </c>
@@ -1600,7 +1607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>43434</v>
       </c>
@@ -1614,7 +1621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>43435</v>
       </c>
@@ -1628,7 +1635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>43441</v>
       </c>
@@ -1642,7 +1649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43444</v>
       </c>
@@ -1656,7 +1663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43446</v>
       </c>
@@ -1670,7 +1677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43447</v>
       </c>
@@ -1684,7 +1691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43448</v>
       </c>
@@ -1698,7 +1705,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43448</v>
       </c>
@@ -1712,7 +1719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43451</v>
       </c>
@@ -1726,7 +1733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>43452</v>
       </c>
@@ -1740,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43453</v>
       </c>
@@ -1754,7 +1761,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43455</v>
       </c>
@@ -1768,7 +1775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>43455</v>
       </c>
@@ -1782,7 +1789,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>43458</v>
       </c>
@@ -1796,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>43458</v>
       </c>
@@ -1810,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>43458</v>
       </c>
@@ -1824,7 +1831,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>43460</v>
       </c>
@@ -1838,7 +1845,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>43462</v>
       </c>
@@ -1852,7 +1859,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>43463</v>
       </c>
@@ -1866,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>43463</v>
       </c>
@@ -1880,7 +1887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>43464</v>
       </c>
@@ -1894,9 +1901,9 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>43102</v>
+        <v>43467</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
@@ -1908,9 +1915,9 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>43103</v>
+        <v>43468</v>
       </c>
       <c r="B90" t="s">
         <v>3</v>
@@ -1922,9 +1929,9 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>43104</v>
+        <v>43469</v>
       </c>
       <c r="B91" t="s">
         <v>3</v>
@@ -1936,9 +1943,9 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>43110</v>
+        <v>43475</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
@@ -1950,9 +1957,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>43110</v>
+        <v>43475</v>
       </c>
       <c r="B93" t="s">
         <v>3</v>
@@ -1964,9 +1971,9 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>43116</v>
+        <v>43481</v>
       </c>
       <c r="B94" t="s">
         <v>3</v>
@@ -1976,6 +1983,34 @@
       </c>
       <c r="D94">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>43499</v>
+      </c>
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" t="s">
+        <v>72</v>
+      </c>
+      <c r="D95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>43500</v>
+      </c>
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>73</v>
+      </c>
+      <c r="D96">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed edit-bug, added comments to code
added work hours
</commit_message>
<xml_diff>
--- a/Organisatorisches/Arbeitszeiten.xlsx
+++ b/Organisatorisches/Arbeitszeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Schule\Diplomarbeit\Ruderverein_ISTER\1819-5ahif-da-ruderverein-ister-dreamteam\Organisatorisches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FEC7AE-7683-45B4-AF82-FF3BAC908597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578A5D74-3A88-4153-8864-F329F54E6EED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6960" xr2:uid="{B5A97CFA-7350-44BD-8E9B-90279A779877}"/>
   </bookViews>
@@ -257,7 +257,7 @@
     <t>Background Images erledigt</t>
   </si>
   <si>
-    <t>Login Form</t>
+    <t>Login Form, Commenting Code</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +713,7 @@
       </c>
       <c r="H3">
         <f>SUMIF(B2:B201,"Daniel",D2:D201)</f>
-        <v>197.5</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2043,7 +2043,7 @@
         <v>75</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>